<commit_message>
Updating crop parameter values in templates
Removing weird winter canola from crop parameters
</commit_message>
<xml_diff>
--- a/static/TemplateMetAndDepletionNodes.xlsx
+++ b/static/TemplateMetAndDepletionNodes.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\USBR_Ag_Demands_Project\CAT_Basins\SanAngeloTX\et_demands_py\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\USBR_Ag_Demands_Project\CAT_Basins\et-demands\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24195" windowHeight="9840" tabRatio="930" firstSheet="1" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26805" windowHeight="13320" tabRatio="930" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="34" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <sheet name="MeanCuttings" sheetId="35" r:id="rId14"/>
     <sheet name="copy_et_cells_crops" sheetId="53" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="152511" calcOnSave="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="518">
   <si>
     <t>Decimal Latitude</t>
   </si>
@@ -1503,9 +1503,6 @@
   </si>
   <si>
     <t>c6</t>
-  </si>
-  <si>
-    <t>Winter Canola</t>
   </si>
   <si>
     <t>MET Data Path</t>
@@ -2080,6 +2077,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2122,7 +2120,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2441,10 +2438,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>415</v>
       </c>
-      <c r="B1" s="51"/>
+      <c r="B1" s="52"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
@@ -2710,7 +2707,7 @@
         <v>214033</v>
       </c>
       <c r="B2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C2" s="15">
         <v>9.673652574544116</v>
@@ -2918,7 +2915,7 @@
         <v>214033</v>
       </c>
       <c r="B2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C2" s="15">
         <v>-4.9861925974232246</v>
@@ -3133,7 +3130,7 @@
         <v>214033</v>
       </c>
       <c r="B3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C3" s="15">
         <v>2</v>
@@ -3474,7 +3471,7 @@
         <v>214033</v>
       </c>
       <c r="B3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C3" s="15">
         <v>2</v>
@@ -3747,7 +3744,7 @@
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
@@ -3760,15 +3757,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="63" t="s">
         <v>347</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="65"/>
       <c r="H1" s="22" t="s">
         <v>348</v>
       </c>
@@ -3809,10 +3806,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>509</v>
+      </c>
+      <c r="B3" t="s">
         <v>510</v>
-      </c>
-      <c r="B3" t="s">
-        <v>511</v>
       </c>
       <c r="C3" s="30">
         <v>35.625555555555557</v>
@@ -4477,7 +4474,7 @@
         <v>413</v>
       </c>
       <c r="B4" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C4" t="s">
         <v>386</v>
@@ -4746,7 +4743,7 @@
         <v>414</v>
       </c>
       <c r="B5" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C5" t="s">
         <v>386</v>
@@ -5042,10 +5039,10 @@
         <v>25695</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>449</v>
+      </c>
+      <c r="E1" s="46" t="s">
         <v>450</v>
-      </c>
-      <c r="E1" s="46" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="66.599999999999994" x14ac:dyDescent="0.3">
@@ -5059,10 +5056,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="12" t="s">
+        <v>451</v>
+      </c>
+      <c r="E2" s="47" t="s">
         <v>452</v>
-      </c>
-      <c r="E2" s="47" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="53.45" x14ac:dyDescent="0.3">
@@ -5076,10 +5073,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="18" t="s">
+        <v>453</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>454</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="76.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -5096,13 +5093,13 @@
         <v>0</v>
       </c>
       <c r="E4" s="48" t="s">
+        <v>455</v>
+      </c>
+      <c r="F4" s="53" t="s">
         <v>456</v>
       </c>
-      <c r="F4" s="52" t="s">
-        <v>457</v>
-      </c>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
       <c r="I4" s="38"/>
       <c r="J4" s="38"/>
     </row>
@@ -5114,7 +5111,7 @@
       <c r="C5" s="43"/>
       <c r="D5" s="43"/>
       <c r="E5" s="12" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
@@ -5129,12 +5126,12 @@
       </c>
       <c r="D6" s="43"/>
       <c r="E6" s="12" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="39" x14ac:dyDescent="0.25">
       <c r="A7" s="45" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B7" s="49" t="s">
         <v>234</v>
@@ -5144,7 +5141,7 @@
       </c>
       <c r="D7" s="45"/>
       <c r="E7" s="12" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="40.15" x14ac:dyDescent="0.3">
@@ -5155,11 +5152,11 @@
         <v>1</v>
       </c>
       <c r="C8" s="45" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D8" s="43"/>
       <c r="E8" s="12" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="40.15" x14ac:dyDescent="0.3">
@@ -5170,323 +5167,323 @@
         <v>20</v>
       </c>
       <c r="C9" s="45" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D9" s="45" t="s">
+        <v>462</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>463</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="42" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B10" s="41" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C10" s="42" t="s">
         <v>310</v>
       </c>
       <c r="D10" s="43"/>
       <c r="E10" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="42" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B11" s="41" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C11" s="42" t="s">
         <v>308</v>
       </c>
       <c r="D11" s="43"/>
       <c r="E11" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="42" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C12" s="42" t="s">
         <v>309</v>
       </c>
       <c r="D12" s="43"/>
       <c r="E12" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="42" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B13" s="41" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C13" s="42" t="s">
         <v>313</v>
       </c>
       <c r="D13" s="43"/>
       <c r="E13" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="42" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B14" s="41" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C14" s="42" t="s">
         <v>314</v>
       </c>
       <c r="D14" s="43"/>
       <c r="E14" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="42" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C15" s="42" t="s">
         <v>315</v>
       </c>
       <c r="D15" s="43"/>
       <c r="E15" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="42" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C16" s="42" t="s">
         <v>316</v>
       </c>
       <c r="D16" s="43"/>
       <c r="E16" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="42" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B17" s="41" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C17" s="42" t="s">
         <v>311</v>
       </c>
       <c r="D17" s="43"/>
       <c r="E17" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="42" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B18" s="41" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C18" s="43" t="s">
         <v>312</v>
       </c>
       <c r="D18" s="43"/>
       <c r="E18" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="42" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C19" s="43" t="s">
         <v>359</v>
       </c>
       <c r="D19" s="43"/>
       <c r="E19" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="42" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C20" s="42" t="s">
         <v>306</v>
       </c>
       <c r="D20" s="43"/>
       <c r="E20" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="42" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B21" s="41" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C21" s="42" t="s">
         <v>307</v>
       </c>
       <c r="D21" s="43"/>
       <c r="E21" s="12" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B22" s="41" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="12" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B23" s="41" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D23" s="43"/>
       <c r="E23" s="12" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B24" s="41" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D24" s="43"/>
       <c r="E24" s="12" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B25" s="41"/>
       <c r="C25" s="43"/>
       <c r="D25" s="43"/>
       <c r="E25" s="12" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B26" s="41"/>
       <c r="C26" s="43"/>
       <c r="D26" s="43"/>
       <c r="E26" s="12" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B27" s="41"/>
       <c r="C27" s="43"/>
       <c r="D27" s="43"/>
       <c r="E27" s="12" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B28" s="41"/>
       <c r="C28" s="43"/>
       <c r="D28" s="43"/>
       <c r="E28" s="12" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B29" s="41"/>
       <c r="C29" s="43"/>
       <c r="D29" s="43"/>
       <c r="E29" s="12" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A30" s="42" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B30" s="41" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="12" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A31" s="42" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B31" s="41" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D31" s="43"/>
       <c r="E31" s="12" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5494,188 +5491,188 @@
         <v>1</v>
       </c>
       <c r="B32" s="41" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C32" s="43"/>
       <c r="D32" s="43"/>
       <c r="E32" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B33" s="41" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C33" s="43"/>
       <c r="D33" s="43"/>
       <c r="E33" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B34" s="41" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C34" s="43"/>
       <c r="D34" s="43"/>
       <c r="E34" s="12" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C35" s="45" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D35" s="45"/>
       <c r="E35" s="12" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B36" s="41" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="12" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B37" s="41" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="12" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B38" s="41" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="12" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B39" s="41" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="12" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B40" s="41" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="12" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B41" s="41" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="12" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B42" s="41" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="12" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B43" s="41" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="12" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B44" s="41" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="12" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
   </sheetData>
@@ -6223,7 +6220,7 @@
         <v>9999</v>
       </c>
       <c r="B2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C2" t="s">
         <v>388</v>
@@ -6252,7 +6249,7 @@
         <v>9999</v>
       </c>
       <c r="B3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C3" t="s">
         <v>417</v>
@@ -6281,7 +6278,7 @@
         <v>9999</v>
       </c>
       <c r="B4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C4" t="s">
         <v>418</v>
@@ -6310,7 +6307,7 @@
         <v>9999</v>
       </c>
       <c r="B5" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C5" t="s">
         <v>419</v>
@@ -6339,7 +6336,7 @@
         <v>9999</v>
       </c>
       <c r="B6" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C6" t="s">
         <v>420</v>
@@ -6368,7 +6365,7 @@
         <v>9999</v>
       </c>
       <c r="B7" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C7" t="s">
         <v>389</v>
@@ -6397,7 +6394,7 @@
         <v>9999</v>
       </c>
       <c r="B8" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C8" t="s">
         <v>119</v>
@@ -6426,7 +6423,7 @@
         <v>9999</v>
       </c>
       <c r="B9" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C9" t="s">
         <v>421</v>
@@ -6455,7 +6452,7 @@
         <v>9999</v>
       </c>
       <c r="B10" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C10" t="s">
         <v>422</v>
@@ -6484,7 +6481,7 @@
         <v>9999</v>
       </c>
       <c r="B11" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C11" t="s">
         <v>390</v>
@@ -6513,7 +6510,7 @@
         <v>9999</v>
       </c>
       <c r="B12" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C12" t="s">
         <v>391</v>
@@ -6542,7 +6539,7 @@
         <v>9999</v>
       </c>
       <c r="B13" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C13" t="s">
         <v>392</v>
@@ -6571,7 +6568,7 @@
         <v>9999</v>
       </c>
       <c r="B14" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C14" t="s">
         <v>393</v>
@@ -6600,7 +6597,7 @@
         <v>9999</v>
       </c>
       <c r="B15" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C15" t="s">
         <v>394</v>
@@ -6629,7 +6626,7 @@
         <v>9999</v>
       </c>
       <c r="B16" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C16" t="s">
         <v>395</v>
@@ -6658,7 +6655,7 @@
         <v>9999</v>
       </c>
       <c r="B17" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C17" t="s">
         <v>396</v>
@@ -6687,7 +6684,7 @@
         <v>9999</v>
       </c>
       <c r="B18" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C18" t="s">
         <v>397</v>
@@ -6716,7 +6713,7 @@
         <v>9999</v>
       </c>
       <c r="B19" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C19" t="s">
         <v>398</v>
@@ -6745,7 +6742,7 @@
         <v>9999</v>
       </c>
       <c r="B20" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C20" t="s">
         <v>399</v>
@@ -6774,7 +6771,7 @@
         <v>9999</v>
       </c>
       <c r="B21" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C21" t="s">
         <v>400</v>
@@ -6803,7 +6800,7 @@
         <v>9999</v>
       </c>
       <c r="B22" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C22" t="s">
         <v>401</v>
@@ -6832,7 +6829,7 @@
         <v>9999</v>
       </c>
       <c r="B23" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C23" t="s">
         <v>402</v>
@@ -6861,7 +6858,7 @@
         <v>9999</v>
       </c>
       <c r="B24" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C24" t="s">
         <v>403</v>
@@ -6890,7 +6887,7 @@
         <v>9999</v>
       </c>
       <c r="B25" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C25" t="s">
         <v>404</v>
@@ -6919,7 +6916,7 @@
         <v>9999</v>
       </c>
       <c r="B26" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C26" t="s">
         <v>118</v>
@@ -6948,7 +6945,7 @@
         <v>9999</v>
       </c>
       <c r="B27" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C27" t="s">
         <v>405</v>
@@ -6977,7 +6974,7 @@
         <v>9999</v>
       </c>
       <c r="B28" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C28" t="s">
         <v>406</v>
@@ -7006,7 +7003,7 @@
         <v>9999</v>
       </c>
       <c r="B29" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C29" t="s">
         <v>339</v>
@@ -7035,7 +7032,7 @@
         <v>9999</v>
       </c>
       <c r="B30" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C30" t="s">
         <v>407</v>
@@ -7064,7 +7061,7 @@
         <v>9999</v>
       </c>
       <c r="B31" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C31" t="s">
         <v>408</v>
@@ -7093,7 +7090,7 @@
         <v>9999</v>
       </c>
       <c r="B32" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C32" t="s">
         <v>338</v>
@@ -7122,7 +7119,7 @@
         <v>9999</v>
       </c>
       <c r="B33" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C33" t="s">
         <v>409</v>
@@ -7151,7 +7148,7 @@
         <v>9999</v>
       </c>
       <c r="B34" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C34" t="s">
         <v>410</v>
@@ -7180,7 +7177,7 @@
         <v>9999</v>
       </c>
       <c r="B35" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C35" t="s">
         <v>423</v>
@@ -7209,7 +7206,7 @@
         <v>9999</v>
       </c>
       <c r="B36" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C36" t="s">
         <v>424</v>
@@ -7238,7 +7235,7 @@
         <v>9999</v>
       </c>
       <c r="B37" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C37" t="s">
         <v>159</v>
@@ -7267,7 +7264,7 @@
         <v>9999</v>
       </c>
       <c r="B38" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C38" t="s">
         <v>337</v>
@@ -7296,7 +7293,7 @@
         <v>9999</v>
       </c>
       <c r="B39" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C39" t="s">
         <v>300</v>
@@ -7325,7 +7322,7 @@
         <v>9999</v>
       </c>
       <c r="B40" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C40" t="s">
         <v>411</v>
@@ -7354,7 +7351,7 @@
         <v>9999</v>
       </c>
       <c r="B41" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C41" t="s">
         <v>191</v>
@@ -7383,7 +7380,7 @@
         <v>9999</v>
       </c>
       <c r="B42" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C42" t="s">
         <v>412</v>
@@ -7412,7 +7409,7 @@
         <v>9999</v>
       </c>
       <c r="B43" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C43" t="s">
         <v>116</v>
@@ -7441,7 +7438,7 @@
         <v>9999</v>
       </c>
       <c r="B44" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C44" t="s">
         <v>117</v>
@@ -7470,7 +7467,7 @@
         <v>9999</v>
       </c>
       <c r="B45" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C45" t="s">
         <v>25</v>
@@ -7702,10 +7699,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>509</v>
+      </c>
+      <c r="B2" t="s">
         <v>510</v>
-      </c>
-      <c r="B2" t="s">
-        <v>511</v>
       </c>
       <c r="C2">
         <v>214033</v>
@@ -8364,10 +8361,10 @@
     </row>
     <row r="4" spans="1:89" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>509</v>
+      </c>
+      <c r="B4" t="s">
         <v>510</v>
-      </c>
-      <c r="B4" t="s">
-        <v>511</v>
       </c>
       <c r="C4">
         <v>214033</v>
@@ -8694,7 +8691,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>360</v>
@@ -8711,7 +8708,7 @@
         <v>214033</v>
       </c>
       <c r="C2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D2">
         <v>31.479347590500002</v>
@@ -8726,13 +8723,13 @@
         <v>214033</v>
       </c>
       <c r="H2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="I2">
         <v>214033</v>
       </c>
       <c r="J2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -8789,10 +8786,10 @@
       <c r="BJ2" s="34"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="55" t="s">
         <v>260</v>
       </c>
-      <c r="B3" s="54"/>
+      <c r="B3" s="55"/>
       <c r="C3">
         <v>1</v>
       </c>
@@ -9034,10 +9031,10 @@
       </c>
     </row>
     <row r="4" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="56" t="s">
         <v>261</v>
       </c>
-      <c r="B4" s="55"/>
+      <c r="B4" s="56"/>
       <c r="C4">
         <v>1</v>
       </c>
@@ -9752,7 +9749,7 @@
       <c r="AZ7" s="15">
         <v>0.18</v>
       </c>
-      <c r="BA7" s="65">
+      <c r="BA7" s="51">
         <v>0.18</v>
       </c>
       <c r="BB7" s="15">
@@ -9940,7 +9937,7 @@
       <c r="AZ8" s="15">
         <v>0.18</v>
       </c>
-      <c r="BA8" s="65">
+      <c r="BA8" s="51">
         <v>0.18</v>
       </c>
       <c r="BB8" s="15">
@@ -10128,7 +10125,7 @@
       <c r="AZ9" s="15">
         <v>0.18</v>
       </c>
-      <c r="BA9" s="65">
+      <c r="BA9" s="51">
         <v>0.24</v>
       </c>
       <c r="BB9" s="15">
@@ -10316,7 +10313,7 @@
       <c r="AZ10" s="15">
         <v>0.2</v>
       </c>
-      <c r="BA10" s="65">
+      <c r="BA10" s="51">
         <v>0.34</v>
       </c>
       <c r="BB10" s="15">
@@ -10504,7 +10501,7 @@
       <c r="AZ11" s="15">
         <v>0.28000000000000003</v>
       </c>
-      <c r="BA11" s="65">
+      <c r="BA11" s="51">
         <v>0.48</v>
       </c>
       <c r="BB11" s="15">
@@ -10692,7 +10689,7 @@
       <c r="AZ12" s="15">
         <v>0.42</v>
       </c>
-      <c r="BA12" s="65">
+      <c r="BA12" s="51">
         <v>0.6</v>
       </c>
       <c r="BB12" s="15">
@@ -10880,7 +10877,7 @@
       <c r="AZ13" s="15">
         <v>0.57999999999999996</v>
       </c>
-      <c r="BA13" s="65">
+      <c r="BA13" s="51">
         <v>0.71</v>
       </c>
       <c r="BB13" s="15">
@@ -11068,7 +11065,7 @@
       <c r="AZ14" s="15">
         <v>0.74</v>
       </c>
-      <c r="BA14" s="65">
+      <c r="BA14" s="51">
         <v>0.98</v>
       </c>
       <c r="BB14" s="15">
@@ -11256,7 +11253,7 @@
       <c r="AZ15" s="15">
         <v>0.79999999999999993</v>
       </c>
-      <c r="BA15" s="65">
+      <c r="BA15" s="51">
         <v>1.1399999999999999</v>
       </c>
       <c r="BB15" s="15">
@@ -11444,7 +11441,7 @@
       <c r="AZ16" s="15">
         <v>0.89999999999999991</v>
       </c>
-      <c r="BA16" s="65">
+      <c r="BA16" s="51">
         <v>1.1499999999999999</v>
       </c>
       <c r="BB16" s="15">
@@ -11632,7 +11629,7 @@
       <c r="AZ17" s="15">
         <v>0.99999999999999989</v>
       </c>
-      <c r="BA17" s="65">
+      <c r="BA17" s="51">
         <v>1.1499999999999999</v>
       </c>
       <c r="BB17" s="15">
@@ -11808,7 +11805,7 @@
       <c r="AZ18" s="15">
         <v>1</v>
       </c>
-      <c r="BA18" s="65">
+      <c r="BA18" s="51">
         <v>1.1499999999999999</v>
       </c>
       <c r="BB18" s="15">
@@ -11984,7 +11981,7 @@
       <c r="AZ19" s="15">
         <v>1</v>
       </c>
-      <c r="BA19" s="65">
+      <c r="BA19" s="51">
         <v>1.1499999999999999</v>
       </c>
       <c r="BB19" s="15">
@@ -12160,7 +12157,7 @@
       <c r="AZ20" s="15">
         <v>1</v>
       </c>
-      <c r="BA20" s="65">
+      <c r="BA20" s="51">
         <v>1.1499999999999999</v>
       </c>
       <c r="BB20" s="15">
@@ -12336,7 +12333,7 @@
       <c r="AZ21" s="15">
         <v>1</v>
       </c>
-      <c r="BA21" s="65">
+      <c r="BA21" s="51">
         <v>1.1499999999999999</v>
       </c>
       <c r="BB21" s="15">
@@ -12512,7 +12509,7 @@
       <c r="AZ22" s="15">
         <v>1</v>
       </c>
-      <c r="BA22" s="65">
+      <c r="BA22" s="51">
         <v>1.1499999999999999</v>
       </c>
       <c r="BB22" s="15">
@@ -12688,7 +12685,7 @@
       <c r="AZ23" s="15">
         <v>1</v>
       </c>
-      <c r="BA23" s="65">
+      <c r="BA23" s="51">
         <v>1.1499999999999999</v>
       </c>
       <c r="BB23" s="15">
@@ -12860,7 +12857,7 @@
       <c r="AZ24" s="15">
         <v>1</v>
       </c>
-      <c r="BA24" s="65">
+      <c r="BA24" s="51">
         <v>1.1499999999999999</v>
       </c>
       <c r="BB24" s="15">
@@ -13028,7 +13025,7 @@
       <c r="AZ25" s="15">
         <v>1</v>
       </c>
-      <c r="BA25" s="65">
+      <c r="BA25" s="51">
         <v>1.1499999999999999</v>
       </c>
       <c r="BB25" s="15">
@@ -13194,7 +13191,7 @@
       <c r="AZ26" s="15">
         <v>1</v>
       </c>
-      <c r="BA26" s="65">
+      <c r="BA26" s="51">
         <v>1.06</v>
       </c>
       <c r="BB26" s="15">
@@ -13356,7 +13353,7 @@
       <c r="AZ27" s="15">
         <v>1</v>
       </c>
-      <c r="BA27" s="65">
+      <c r="BA27" s="51">
         <v>0.77</v>
       </c>
       <c r="BB27" s="15">
@@ -13514,7 +13511,7 @@
       <c r="AZ28" s="15">
         <v>1</v>
       </c>
-      <c r="BA28" s="65">
+      <c r="BA28" s="51">
         <v>0.49</v>
       </c>
       <c r="BB28" s="15">
@@ -13664,7 +13661,7 @@
       <c r="AZ29" s="15">
         <v>1</v>
       </c>
-      <c r="BA29" s="65">
+      <c r="BA29" s="51">
         <v>0.45</v>
       </c>
       <c r="BB29" s="15"/>
@@ -13806,7 +13803,7 @@
       <c r="AZ30" s="15">
         <v>0.95</v>
       </c>
-      <c r="BA30" s="65">
+      <c r="BA30" s="51">
         <v>0.45</v>
       </c>
       <c r="BB30" s="15"/>
@@ -13946,7 +13943,7 @@
       <c r="AZ31" s="15">
         <v>0.89999999999999991</v>
       </c>
-      <c r="BA31" s="65">
+      <c r="BA31" s="51">
         <v>0.45</v>
       </c>
       <c r="BB31" s="15"/>
@@ -14076,7 +14073,7 @@
       <c r="AZ32" s="15">
         <v>0.84999999999999987</v>
       </c>
-      <c r="BA32" s="65">
+      <c r="BA32" s="51">
         <v>0.45</v>
       </c>
       <c r="BB32" s="15"/>
@@ -15436,11 +15433,11 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:CI62"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="BG12" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="5" topLeftCell="AO12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="BI22" sqref="BI22"/>
+      <selection pane="bottomRight" activeCell="AQ24" sqref="AQ24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15453,12 +15450,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="58"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="59"/>
       <c r="G1" s="16" t="s">
         <v>122</v>
       </c>
@@ -15468,11 +15465,11 @@
         <f>COUNTIF(C$5:CI$5,"&lt;&gt; ")</f>
         <v>85</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="60" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="62"/>
       <c r="G2" s="16" t="s">
         <v>124</v>
       </c>
@@ -15482,10 +15479,10 @@
         <v>125</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="57" t="s">
         <v>126</v>
       </c>
-      <c r="D3" s="58"/>
+      <c r="D3" s="59"/>
     </row>
     <row r="4" spans="1:87" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -15874,8 +15871,8 @@
       <c r="AO5" s="2">
         <v>-39</v>
       </c>
-      <c r="AP5" s="2">
-        <v>-40</v>
+      <c r="AP5" s="1">
+        <v>40</v>
       </c>
       <c r="AQ5" s="2">
         <v>-41</v>
@@ -16125,9 +16122,7 @@
         <v>1</v>
       </c>
       <c r="AO6" s="2"/>
-      <c r="AP6" s="2">
-        <v>1</v>
-      </c>
+      <c r="AP6" s="1"/>
       <c r="AQ6" s="2"/>
       <c r="AR6" s="2"/>
       <c r="AS6" s="2">
@@ -16356,8 +16351,8 @@
       <c r="AO7" s="2">
         <v>0</v>
       </c>
-      <c r="AP7" s="2">
-        <v>155</v>
+      <c r="AP7" s="1">
+        <v>0</v>
       </c>
       <c r="AQ7" s="2">
         <v>0</v>
@@ -16619,7 +16614,7 @@
       <c r="AO8" s="2">
         <v>1</v>
       </c>
-      <c r="AP8" s="2">
+      <c r="AP8" s="1">
         <v>1</v>
       </c>
       <c r="AQ8" s="2">
@@ -16882,7 +16877,7 @@
       <c r="AO9" s="8">
         <v>2</v>
       </c>
-      <c r="AP9" s="8">
+      <c r="AP9" s="1">
         <v>2</v>
       </c>
       <c r="AQ9" s="8">
@@ -17139,8 +17134,8 @@
       <c r="AO10" s="2">
         <v>1</v>
       </c>
-      <c r="AP10" s="2">
-        <v>1</v>
+      <c r="AP10" s="1">
+        <v>1.2</v>
       </c>
       <c r="AQ10" s="2">
         <v>1</v>
@@ -17402,7 +17397,7 @@
       <c r="AO11" s="2">
         <v>60</v>
       </c>
-      <c r="AP11" s="2">
+      <c r="AP11" s="1">
         <v>60</v>
       </c>
       <c r="AQ11" s="2">
@@ -17663,8 +17658,8 @@
       <c r="AO12" s="2">
         <v>60</v>
       </c>
-      <c r="AP12" s="2">
-        <v>50</v>
+      <c r="AP12" s="1">
+        <v>60</v>
       </c>
       <c r="AQ12" s="2">
         <v>60</v>
@@ -17926,8 +17921,8 @@
       <c r="AO13" s="2">
         <v>0.2</v>
       </c>
-      <c r="AP13" s="2">
-        <v>0.25</v>
+      <c r="AP13" s="1">
+        <v>0.2</v>
       </c>
       <c r="AQ13" s="2">
         <v>0.2</v>
@@ -18189,8 +18184,8 @@
       <c r="AO14" s="2">
         <v>2.5</v>
       </c>
-      <c r="AP14" s="2">
-        <v>1.8</v>
+      <c r="AP14" s="1">
+        <v>1.6</v>
       </c>
       <c r="AQ14" s="2">
         <v>1.4</v>
@@ -18452,7 +18447,7 @@
       <c r="AO15" s="2">
         <v>1.2</v>
       </c>
-      <c r="AP15" s="2">
+      <c r="AP15" s="1">
         <v>1.2</v>
       </c>
       <c r="AQ15" s="2">
@@ -18715,8 +18710,8 @@
       <c r="AO16" s="2">
         <v>0.1</v>
       </c>
-      <c r="AP16" s="2">
-        <v>0.05</v>
+      <c r="AP16" s="1">
+        <v>0.1</v>
       </c>
       <c r="AQ16" s="2">
         <v>0.1</v>
@@ -18978,7 +18973,7 @@
       <c r="AO17" s="2">
         <v>1</v>
       </c>
-      <c r="AP17" s="2">
+      <c r="AP17" s="1">
         <v>1</v>
       </c>
       <c r="AQ17" s="2">
@@ -19241,8 +19236,8 @@
       <c r="AO18" s="2">
         <v>28</v>
       </c>
-      <c r="AP18" s="2">
-        <v>2</v>
+      <c r="AP18" s="1">
+        <v>27</v>
       </c>
       <c r="AQ18" s="2">
         <v>27</v>
@@ -19505,7 +19500,7 @@
         <v>206</v>
       </c>
       <c r="AP19" s="1" t="s">
-        <v>437</v>
+        <v>79</v>
       </c>
       <c r="AQ19" s="1" t="s">
         <v>80</v>
@@ -19755,8 +19750,8 @@
       <c r="AO20" s="2">
         <v>2</v>
       </c>
-      <c r="AP20" s="2">
-        <v>1</v>
+      <c r="AP20" s="1">
+        <v>2</v>
       </c>
       <c r="AQ20" s="2">
         <v>2</v>
@@ -20012,8 +20007,8 @@
       <c r="AO21" s="2">
         <v>2</v>
       </c>
-      <c r="AP21" s="2">
-        <v>3</v>
+      <c r="AP21" s="1">
+        <v>2</v>
       </c>
       <c r="AQ21" s="2">
         <v>3</v>
@@ -20269,7 +20264,9 @@
       <c r="AO22" s="9">
         <v>11</v>
       </c>
-      <c r="AP22" s="9"/>
+      <c r="AP22" s="50">
+        <v>8</v>
+      </c>
       <c r="AQ22" s="9">
         <v>11</v>
       </c>
@@ -20442,11 +20439,9 @@
       <c r="AM23" s="2"/>
       <c r="AN23" s="2"/>
       <c r="AO23" s="2"/>
-      <c r="AP23" s="2">
-        <v>10</v>
-      </c>
+      <c r="AP23" s="1"/>
       <c r="AQ23" s="2">
-        <v>4.833333333333333</v>
+        <v>4.83</v>
       </c>
       <c r="AR23" s="2"/>
       <c r="AS23" s="2"/>
@@ -20605,9 +20600,7 @@
       <c r="AM24" s="2"/>
       <c r="AN24" s="2"/>
       <c r="AO24" s="2"/>
-      <c r="AP24" s="2">
-        <v>0</v>
-      </c>
+      <c r="AP24" s="1"/>
       <c r="AQ24" s="2"/>
       <c r="AR24" s="2"/>
       <c r="AS24" s="2"/>
@@ -20782,9 +20775,7 @@
       <c r="AM25" s="2"/>
       <c r="AN25" s="2"/>
       <c r="AO25" s="2"/>
-      <c r="AP25" s="2">
-        <v>1150</v>
-      </c>
+      <c r="AP25" s="1"/>
       <c r="AQ25" s="2"/>
       <c r="AR25" s="2"/>
       <c r="AS25" s="2"/>
@@ -20953,9 +20944,7 @@
       <c r="AM26" s="2"/>
       <c r="AN26" s="2"/>
       <c r="AO26" s="2"/>
-      <c r="AP26" s="2">
-        <v>2000</v>
-      </c>
+      <c r="AP26" s="1"/>
       <c r="AQ26" s="2"/>
       <c r="AR26" s="2"/>
       <c r="AS26" s="2"/>
@@ -21080,7 +21069,7 @@
       <c r="AM27" s="2"/>
       <c r="AN27" s="2"/>
       <c r="AO27" s="2"/>
-      <c r="AP27" s="2"/>
+      <c r="AP27" s="1"/>
       <c r="AQ27" s="2"/>
       <c r="AR27" s="2"/>
       <c r="AS27" s="2"/>
@@ -21209,7 +21198,9 @@
       <c r="AO28" s="2">
         <v>70</v>
       </c>
-      <c r="AP28" s="2"/>
+      <c r="AP28" s="1">
+        <v>55</v>
+      </c>
       <c r="AQ28" s="2">
         <v>55</v>
       </c>
@@ -21394,7 +21385,9 @@
       <c r="AO29" s="2">
         <v>190</v>
       </c>
-      <c r="AP29" s="2"/>
+      <c r="AP29" s="1">
+        <v>170</v>
+      </c>
       <c r="AQ29" s="2">
         <v>190</v>
       </c>
@@ -21603,8 +21596,8 @@
       <c r="AO30" s="2">
         <v>-4</v>
       </c>
-      <c r="AP30" s="2">
-        <v>-100</v>
+      <c r="AP30" s="1">
+        <v>-4</v>
       </c>
       <c r="AQ30" s="2">
         <v>-4</v>
@@ -21866,8 +21859,8 @@
       <c r="AO31" s="2">
         <v>1</v>
       </c>
-      <c r="AP31" s="2">
-        <v>2</v>
+      <c r="AP31" s="1">
+        <v>1</v>
       </c>
       <c r="AQ31" s="2">
         <v>1</v>
@@ -22049,7 +22042,7 @@
       <c r="AM32" s="2"/>
       <c r="AN32" s="2"/>
       <c r="AO32" s="2"/>
-      <c r="AP32" s="2"/>
+      <c r="AP32" s="1"/>
       <c r="AQ32" s="2"/>
       <c r="AR32" s="2"/>
       <c r="AS32" s="2"/>
@@ -22218,7 +22211,7 @@
       <c r="AO33" s="2">
         <v>58</v>
       </c>
-      <c r="AP33" s="2">
+      <c r="AP33" s="1">
         <v>58</v>
       </c>
       <c r="AQ33" s="2">
@@ -22473,7 +22466,7 @@
       <c r="AO34" s="2">
         <v>72</v>
       </c>
-      <c r="AP34" s="2">
+      <c r="AP34" s="1">
         <v>72</v>
       </c>
       <c r="AQ34" s="2">
@@ -22728,7 +22721,7 @@
       <c r="AO35" s="2">
         <v>83</v>
       </c>
-      <c r="AP35" s="2">
+      <c r="AP35" s="1">
         <v>83</v>
       </c>
       <c r="AQ35" s="2">

</xml_diff>

<commit_message>
Support for monthly ETo/ETr ratios by ETCell closes #11
ETo/ETr ratios are set in a static text file called EToRatiosMon.txt
that has a similar structure to the TMinMon and TMaxMon tabs in the
excel file.
</commit_message>
<xml_diff>
--- a/static/TemplateMetAndDepletionNodes.xlsx
+++ b/static/TemplateMetAndDepletionNodes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26805" windowHeight="13320" tabRatio="930" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26805" windowHeight="13320" tabRatio="930" firstSheet="4" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="34" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="WindMon" sheetId="24" r:id="rId12"/>
     <sheet name="KoMon" sheetId="25" r:id="rId13"/>
     <sheet name="MeanCuttings" sheetId="35" r:id="rId14"/>
-    <sheet name="copy_et_cells_crops" sheetId="53" r:id="rId15"/>
+    <sheet name="EToRatiosMon" sheetId="54" r:id="rId15"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="513">
   <si>
     <t>Decimal Latitude</t>
   </si>
@@ -1352,9 +1352,6 @@
     <t>HUC_10</t>
   </si>
   <si>
-    <t>OK1504</t>
-  </si>
-  <si>
     <t>mps</t>
   </si>
   <si>
@@ -1433,12 +1430,6 @@
     <t>Triticale</t>
   </si>
   <si>
-    <t>Washita_1113030205</t>
-  </si>
-  <si>
-    <t>Washita_1113030207</t>
-  </si>
-  <si>
     <t>Inventory of Upper Washita Basin Study Penman Monteith Mapping and Parameter Worksheets</t>
   </si>
   <si>
@@ -1698,12 +1689,6 @@
   </si>
   <si>
     <t>NIRFraction</t>
-  </si>
-  <si>
-    <t>Cobb Creek</t>
-  </si>
-  <si>
-    <t>City of Anadarko-Washita River</t>
   </si>
   <si>
     <t>ETo</t>
@@ -2439,7 +2424,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="52" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="B1" s="52"/>
     </row>
@@ -2649,7 +2634,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2707,7 +2692,7 @@
         <v>214033</v>
       </c>
       <c r="B2" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="C2" s="15">
         <v>9.673652574544116</v>
@@ -2915,7 +2900,7 @@
         <v>214033</v>
       </c>
       <c r="B2" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="C2" s="15">
         <v>-4.9861925974232246</v>
@@ -3078,7 +3063,7 @@
         <v>112</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -3130,7 +3115,7 @@
         <v>214033</v>
       </c>
       <c r="B3" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="C3" s="15">
         <v>2</v>
@@ -3471,7 +3456,7 @@
         <v>214033</v>
       </c>
       <c r="B3" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="C3" s="15">
         <v>2</v>
@@ -3806,10 +3791,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="B3" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="C3" s="30">
         <v>35.625555555555557</v>
@@ -3921,1090 +3906,104 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CK5"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:89" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2">
-        <v>85</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="H2">
-        <v>4</v>
-      </c>
-      <c r="I2">
-        <v>5</v>
-      </c>
-      <c r="J2">
-        <v>6</v>
-      </c>
-      <c r="K2">
-        <v>7</v>
-      </c>
-      <c r="L2">
-        <v>8</v>
-      </c>
-      <c r="M2">
-        <v>9</v>
-      </c>
-      <c r="N2">
-        <v>10</v>
-      </c>
-      <c r="O2">
-        <v>11</v>
-      </c>
-      <c r="P2">
-        <v>12</v>
-      </c>
-      <c r="Q2">
-        <v>13</v>
-      </c>
-      <c r="R2">
-        <v>14</v>
-      </c>
-      <c r="S2">
-        <v>15</v>
-      </c>
-      <c r="T2">
-        <v>16</v>
-      </c>
-      <c r="U2">
-        <v>17</v>
-      </c>
-      <c r="V2">
-        <v>18</v>
-      </c>
-      <c r="W2">
-        <v>19</v>
-      </c>
-      <c r="X2">
-        <v>20</v>
-      </c>
-      <c r="Y2">
-        <v>21</v>
-      </c>
-      <c r="Z2">
-        <v>22</v>
-      </c>
-      <c r="AA2">
-        <v>23</v>
-      </c>
-      <c r="AB2">
-        <v>24</v>
-      </c>
-      <c r="AC2">
-        <v>25</v>
-      </c>
-      <c r="AD2">
-        <v>26</v>
-      </c>
-      <c r="AE2">
-        <v>27</v>
-      </c>
-      <c r="AF2">
-        <v>28</v>
-      </c>
-      <c r="AG2">
-        <v>29</v>
-      </c>
-      <c r="AH2">
-        <v>30</v>
-      </c>
-      <c r="AI2">
-        <v>31</v>
-      </c>
-      <c r="AJ2">
-        <v>32</v>
-      </c>
-      <c r="AK2">
-        <v>33</v>
-      </c>
-      <c r="AL2">
-        <v>34</v>
-      </c>
-      <c r="AM2">
-        <v>35</v>
-      </c>
-      <c r="AN2">
-        <v>36</v>
-      </c>
-      <c r="AO2">
-        <v>37</v>
-      </c>
-      <c r="AP2">
-        <v>38</v>
-      </c>
-      <c r="AQ2">
-        <v>39</v>
-      </c>
-      <c r="AR2">
-        <v>40</v>
-      </c>
-      <c r="AS2">
-        <v>41</v>
-      </c>
-      <c r="AT2">
-        <v>42</v>
-      </c>
-      <c r="AU2">
-        <v>43</v>
-      </c>
-      <c r="AV2">
-        <v>44</v>
-      </c>
-      <c r="AW2">
-        <v>45</v>
-      </c>
-      <c r="AX2">
-        <v>46</v>
-      </c>
-      <c r="AY2">
-        <v>47</v>
-      </c>
-      <c r="AZ2">
-        <v>48</v>
-      </c>
-      <c r="BA2">
-        <v>49</v>
-      </c>
-      <c r="BB2">
-        <v>50</v>
-      </c>
-      <c r="BC2">
-        <v>51</v>
-      </c>
-      <c r="BD2">
-        <v>52</v>
-      </c>
-      <c r="BE2">
-        <v>53</v>
-      </c>
-      <c r="BF2">
-        <v>54</v>
-      </c>
-      <c r="BG2">
-        <v>55</v>
-      </c>
-      <c r="BH2">
-        <v>56</v>
-      </c>
-      <c r="BI2">
-        <v>57</v>
-      </c>
-      <c r="BJ2">
-        <v>58</v>
-      </c>
-      <c r="BK2">
-        <v>59</v>
-      </c>
-      <c r="BL2">
-        <v>60</v>
-      </c>
-      <c r="BM2">
-        <v>61</v>
-      </c>
-      <c r="BN2">
-        <v>62</v>
-      </c>
-      <c r="BO2">
-        <v>63</v>
-      </c>
-      <c r="BP2">
-        <v>64</v>
-      </c>
-      <c r="BQ2">
-        <v>65</v>
-      </c>
-      <c r="BR2">
-        <v>66</v>
-      </c>
-      <c r="BS2">
-        <v>67</v>
-      </c>
-      <c r="BT2">
-        <v>68</v>
-      </c>
-      <c r="BU2">
-        <v>69</v>
-      </c>
-      <c r="BV2">
-        <v>70</v>
-      </c>
-      <c r="BW2">
-        <v>71</v>
-      </c>
-      <c r="BX2">
-        <v>72</v>
-      </c>
-      <c r="BY2">
-        <v>73</v>
-      </c>
-      <c r="BZ2">
-        <v>74</v>
-      </c>
-      <c r="CA2">
-        <v>75</v>
-      </c>
-      <c r="CB2">
-        <v>76</v>
-      </c>
-      <c r="CC2">
-        <v>77</v>
-      </c>
-      <c r="CD2">
-        <v>78</v>
-      </c>
-      <c r="CE2">
-        <v>79</v>
-      </c>
-      <c r="CF2">
-        <v>80</v>
-      </c>
-      <c r="CG2">
-        <v>81</v>
-      </c>
-      <c r="CH2">
-        <v>82</v>
-      </c>
-      <c r="CI2">
-        <v>83</v>
-      </c>
-      <c r="CJ2">
-        <v>84</v>
-      </c>
-      <c r="CK2">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:89" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" t="s">
-        <v>46</v>
-      </c>
-      <c r="L3" t="s">
-        <v>47</v>
-      </c>
-      <c r="M3" t="s">
-        <v>48</v>
-      </c>
-      <c r="N3" t="s">
-        <v>49</v>
-      </c>
-      <c r="O3" t="s">
-        <v>50</v>
-      </c>
-      <c r="P3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>52</v>
-      </c>
-      <c r="R3" t="s">
-        <v>53</v>
-      </c>
-      <c r="S3" t="s">
-        <v>54</v>
-      </c>
-      <c r="T3" t="s">
-        <v>55</v>
-      </c>
-      <c r="U3" t="s">
-        <v>56</v>
-      </c>
-      <c r="V3" t="s">
-        <v>57</v>
-      </c>
-      <c r="W3" t="s">
-        <v>58</v>
-      </c>
-      <c r="X3" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>65</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>69</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>72</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>75</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>78</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>79</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>80</v>
-      </c>
-      <c r="AT3" t="s">
-        <v>81</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>82</v>
-      </c>
-      <c r="AV3" t="s">
-        <v>83</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX3" t="s">
-        <v>85</v>
-      </c>
-      <c r="AY3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>87</v>
-      </c>
-      <c r="BA3" t="s">
-        <v>88</v>
-      </c>
-      <c r="BB3" t="s">
-        <v>89</v>
-      </c>
-      <c r="BC3" t="s">
-        <v>90</v>
-      </c>
-      <c r="BD3" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE3" t="s">
-        <v>92</v>
-      </c>
-      <c r="BF3" t="s">
-        <v>93</v>
-      </c>
-      <c r="BG3" t="s">
-        <v>94</v>
-      </c>
-      <c r="BH3" t="s">
-        <v>95</v>
-      </c>
-      <c r="BI3" t="s">
-        <v>96</v>
-      </c>
-      <c r="BJ3" t="s">
-        <v>119</v>
-      </c>
-      <c r="BK3" t="s">
-        <v>120</v>
-      </c>
-      <c r="BL3" t="s">
-        <v>159</v>
-      </c>
-      <c r="BM3" t="s">
-        <v>301</v>
-      </c>
-      <c r="BN3" t="s">
-        <v>302</v>
-      </c>
-      <c r="BO3" t="s">
-        <v>303</v>
-      </c>
-      <c r="BP3" t="s">
-        <v>304</v>
-      </c>
-      <c r="BQ3" t="s">
-        <v>336</v>
-      </c>
-      <c r="BR3" t="s">
-        <v>337</v>
-      </c>
-      <c r="BS3" t="s">
-        <v>338</v>
-      </c>
-      <c r="BT3" t="s">
-        <v>339</v>
-      </c>
-      <c r="BU3" t="s">
-        <v>340</v>
-      </c>
-      <c r="BV3" t="s">
-        <v>341</v>
-      </c>
-      <c r="BW3" t="s">
-        <v>342</v>
-      </c>
-      <c r="BX3" t="s">
-        <v>343</v>
-      </c>
-      <c r="BY3" t="s">
-        <v>344</v>
-      </c>
-      <c r="BZ3" t="s">
-        <v>367</v>
-      </c>
-      <c r="CA3" t="s">
-        <v>345</v>
-      </c>
-      <c r="CB3" t="s">
-        <v>346</v>
-      </c>
-      <c r="CC3" t="s">
-        <v>361</v>
-      </c>
-      <c r="CD3" t="s">
-        <v>362</v>
-      </c>
-      <c r="CE3" t="s">
-        <v>363</v>
-      </c>
-      <c r="CF3" t="s">
-        <v>364</v>
-      </c>
-      <c r="CG3" t="s">
-        <v>365</v>
-      </c>
-      <c r="CH3" t="s">
-        <v>369</v>
-      </c>
-      <c r="CI3" t="s">
-        <v>370</v>
-      </c>
-      <c r="CJ3" t="s">
-        <v>371</v>
-      </c>
-      <c r="CK3" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="4" spans="1:89" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>413</v>
-      </c>
-      <c r="B4" t="s">
-        <v>502</v>
-      </c>
-      <c r="C4" t="s">
-        <v>386</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>1</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-      <c r="Y4">
-        <v>1</v>
-      </c>
-      <c r="Z4">
-        <v>0</v>
-      </c>
-      <c r="AA4">
-        <v>0</v>
-      </c>
-      <c r="AB4">
-        <v>0</v>
-      </c>
-      <c r="AC4">
-        <v>0</v>
-      </c>
-      <c r="AD4">
-        <v>0</v>
-      </c>
-      <c r="AE4">
-        <v>0</v>
-      </c>
-      <c r="AF4">
-        <v>1</v>
-      </c>
-      <c r="AG4">
-        <v>0</v>
-      </c>
-      <c r="AH4">
-        <v>0</v>
-      </c>
-      <c r="AI4">
-        <v>0</v>
-      </c>
-      <c r="AJ4">
-        <v>0</v>
-      </c>
-      <c r="AK4">
-        <v>0</v>
-      </c>
-      <c r="AL4">
-        <v>0</v>
-      </c>
-      <c r="AM4">
-        <v>0</v>
-      </c>
-      <c r="AN4">
-        <v>1</v>
-      </c>
-      <c r="AO4">
-        <v>0</v>
-      </c>
-      <c r="AP4">
-        <v>0</v>
-      </c>
-      <c r="AQ4">
-        <v>0</v>
-      </c>
-      <c r="AR4">
-        <v>1</v>
-      </c>
-      <c r="AS4">
-        <v>0</v>
-      </c>
-      <c r="AT4">
-        <v>0</v>
-      </c>
-      <c r="AU4">
-        <v>0</v>
-      </c>
-      <c r="AV4">
-        <v>1</v>
-      </c>
-      <c r="AW4">
-        <v>1</v>
-      </c>
-      <c r="AX4">
-        <v>1</v>
-      </c>
-      <c r="AY4">
-        <v>0</v>
-      </c>
-      <c r="AZ4">
-        <v>0</v>
-      </c>
-      <c r="BA4">
-        <v>0</v>
-      </c>
-      <c r="BB4">
-        <v>0</v>
-      </c>
-      <c r="BC4">
-        <v>0</v>
-      </c>
-      <c r="BD4">
-        <v>0</v>
-      </c>
-      <c r="BE4">
-        <v>0</v>
-      </c>
-      <c r="BF4">
-        <v>0</v>
-      </c>
-      <c r="BG4">
-        <v>0</v>
-      </c>
-      <c r="BH4">
-        <v>0</v>
-      </c>
-      <c r="BI4">
-        <v>0</v>
-      </c>
-      <c r="BJ4">
-        <v>1</v>
-      </c>
-      <c r="BK4">
-        <v>0</v>
-      </c>
-      <c r="BL4">
-        <v>1</v>
-      </c>
-      <c r="BM4">
-        <v>0</v>
-      </c>
-      <c r="BN4">
-        <v>0</v>
-      </c>
-      <c r="BO4">
-        <v>0</v>
-      </c>
-      <c r="BP4">
-        <v>0</v>
-      </c>
-      <c r="BQ4">
-        <v>0</v>
-      </c>
-      <c r="BR4">
-        <v>1</v>
-      </c>
-      <c r="BS4">
-        <v>1</v>
-      </c>
-      <c r="BT4">
-        <v>1</v>
-      </c>
-      <c r="BU4">
-        <v>0</v>
-      </c>
-      <c r="BV4">
-        <v>0</v>
-      </c>
-      <c r="BW4">
-        <v>0</v>
-      </c>
-      <c r="BX4">
-        <v>0</v>
-      </c>
-      <c r="BY4">
-        <v>0</v>
-      </c>
-      <c r="BZ4">
-        <v>1</v>
-      </c>
-      <c r="CA4">
-        <v>0</v>
-      </c>
-      <c r="CB4">
-        <v>0</v>
-      </c>
-      <c r="CC4">
-        <v>0</v>
-      </c>
-      <c r="CD4">
-        <v>0</v>
-      </c>
-      <c r="CE4">
-        <v>0</v>
-      </c>
-      <c r="CF4">
-        <v>0</v>
-      </c>
-      <c r="CG4">
-        <v>0</v>
-      </c>
-      <c r="CH4">
-        <v>0</v>
-      </c>
-      <c r="CI4">
-        <v>0</v>
-      </c>
-      <c r="CJ4">
-        <v>0</v>
-      </c>
-      <c r="CK4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:89" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>414</v>
-      </c>
-      <c r="B5" t="s">
-        <v>503</v>
-      </c>
-      <c r="C5" t="s">
-        <v>386</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>1</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>1</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>1</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
-      <c r="Y5">
-        <v>1</v>
-      </c>
-      <c r="Z5">
-        <v>0</v>
-      </c>
-      <c r="AA5">
-        <v>0</v>
-      </c>
-      <c r="AB5">
-        <v>0</v>
-      </c>
-      <c r="AC5">
-        <v>0</v>
-      </c>
-      <c r="AD5">
-        <v>0</v>
-      </c>
-      <c r="AE5">
-        <v>0</v>
-      </c>
-      <c r="AF5">
-        <v>1</v>
-      </c>
-      <c r="AG5">
-        <v>0</v>
-      </c>
-      <c r="AH5">
-        <v>0</v>
-      </c>
-      <c r="AI5">
-        <v>0</v>
-      </c>
-      <c r="AJ5">
-        <v>0</v>
-      </c>
-      <c r="AK5">
-        <v>0</v>
-      </c>
-      <c r="AL5">
-        <v>0</v>
-      </c>
-      <c r="AM5">
-        <v>0</v>
-      </c>
-      <c r="AN5">
-        <v>0</v>
-      </c>
-      <c r="AO5">
-        <v>0</v>
-      </c>
-      <c r="AP5">
-        <v>0</v>
-      </c>
-      <c r="AQ5">
-        <v>0</v>
-      </c>
-      <c r="AR5">
-        <v>1</v>
-      </c>
-      <c r="AS5">
-        <v>0</v>
-      </c>
-      <c r="AT5">
-        <v>0</v>
-      </c>
-      <c r="AU5">
-        <v>0</v>
-      </c>
-      <c r="AV5">
-        <v>1</v>
-      </c>
-      <c r="AW5">
-        <v>1</v>
-      </c>
-      <c r="AX5">
-        <v>1</v>
-      </c>
-      <c r="AY5">
-        <v>0</v>
-      </c>
-      <c r="AZ5">
-        <v>0</v>
-      </c>
-      <c r="BA5">
-        <v>0</v>
-      </c>
-      <c r="BB5">
-        <v>0</v>
-      </c>
-      <c r="BC5">
-        <v>0</v>
-      </c>
-      <c r="BD5">
-        <v>0</v>
-      </c>
-      <c r="BE5">
-        <v>0</v>
-      </c>
-      <c r="BF5">
-        <v>0</v>
-      </c>
-      <c r="BG5">
-        <v>0</v>
-      </c>
-      <c r="BH5">
-        <v>0</v>
-      </c>
-      <c r="BI5">
-        <v>0</v>
-      </c>
-      <c r="BJ5">
-        <v>1</v>
-      </c>
-      <c r="BK5">
-        <v>0</v>
-      </c>
-      <c r="BL5">
-        <v>1</v>
-      </c>
-      <c r="BM5">
-        <v>0</v>
-      </c>
-      <c r="BN5">
-        <v>0</v>
-      </c>
-      <c r="BO5">
-        <v>0</v>
-      </c>
-      <c r="BP5">
-        <v>0</v>
-      </c>
-      <c r="BQ5">
-        <v>0</v>
-      </c>
-      <c r="BR5">
-        <v>1</v>
-      </c>
-      <c r="BS5">
-        <v>1</v>
-      </c>
-      <c r="BT5">
-        <v>0</v>
-      </c>
-      <c r="BU5">
-        <v>0</v>
-      </c>
-      <c r="BV5">
-        <v>0</v>
-      </c>
-      <c r="BW5">
-        <v>0</v>
-      </c>
-      <c r="BX5">
-        <v>0</v>
-      </c>
-      <c r="BY5">
-        <v>0</v>
-      </c>
-      <c r="BZ5">
-        <v>0</v>
-      </c>
-      <c r="CA5">
-        <v>0</v>
-      </c>
-      <c r="CB5">
-        <v>0</v>
-      </c>
-      <c r="CC5">
-        <v>0</v>
-      </c>
-      <c r="CD5">
-        <v>0</v>
-      </c>
-      <c r="CE5">
-        <v>0</v>
-      </c>
-      <c r="CF5">
-        <v>0</v>
-      </c>
-      <c r="CG5">
-        <v>0</v>
-      </c>
-      <c r="CH5">
-        <v>0</v>
-      </c>
-      <c r="CI5">
-        <v>0</v>
-      </c>
-      <c r="CJ5">
-        <v>0</v>
-      </c>
-      <c r="CK5">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I1" t="s">
+        <v>106</v>
+      </c>
+      <c r="J1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" t="s">
+        <v>109</v>
+      </c>
+      <c r="M1" t="s">
+        <v>110</v>
+      </c>
+      <c r="N1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>214033</v>
+      </c>
+      <c r="B2" t="s">
+        <v>505</v>
+      </c>
+      <c r="C2" s="15">
+        <v>1</v>
+      </c>
+      <c r="D2" s="15">
+        <v>1</v>
+      </c>
+      <c r="E2" s="15">
+        <v>1</v>
+      </c>
+      <c r="F2" s="15">
+        <v>1</v>
+      </c>
+      <c r="G2" s="15">
+        <v>1</v>
+      </c>
+      <c r="H2" s="15">
+        <v>1</v>
+      </c>
+      <c r="I2" s="15">
+        <v>1</v>
+      </c>
+      <c r="J2" s="15">
+        <v>1</v>
+      </c>
+      <c r="K2" s="15">
+        <v>1</v>
+      </c>
+      <c r="L2" s="15">
+        <v>1</v>
+      </c>
+      <c r="M2" s="15">
+        <v>1</v>
+      </c>
+      <c r="N2" s="15">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5039,10 +4038,10 @@
         <v>25695</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="E1" s="46" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="66.599999999999994" x14ac:dyDescent="0.3">
@@ -5056,10 +4055,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="E2" s="47" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="53.45" x14ac:dyDescent="0.3">
@@ -5073,10 +4072,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="76.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -5093,10 +4092,10 @@
         <v>0</v>
       </c>
       <c r="E4" s="48" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="F4" s="53" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="G4" s="54"/>
       <c r="H4" s="54"/>
@@ -5111,7 +4110,7 @@
       <c r="C5" s="43"/>
       <c r="D5" s="43"/>
       <c r="E5" s="12" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
@@ -5126,22 +4125,22 @@
       </c>
       <c r="D6" s="43"/>
       <c r="E6" s="12" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="39" x14ac:dyDescent="0.25">
       <c r="A7" s="45" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="B7" s="49" t="s">
         <v>234</v>
       </c>
       <c r="C7" s="45" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D7" s="45"/>
       <c r="E7" s="12" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="40.15" x14ac:dyDescent="0.3">
@@ -5152,11 +4151,11 @@
         <v>1</v>
       </c>
       <c r="C8" s="45" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="D8" s="43"/>
       <c r="E8" s="12" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="40.15" x14ac:dyDescent="0.3">
@@ -5167,323 +4166,323 @@
         <v>20</v>
       </c>
       <c r="C9" s="45" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="D9" s="45" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="42" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B10" s="41" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="C10" s="42" t="s">
         <v>310</v>
       </c>
       <c r="D10" s="43"/>
       <c r="E10" s="1" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="42" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B11" s="41" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="C11" s="42" t="s">
         <v>308</v>
       </c>
       <c r="D11" s="43"/>
       <c r="E11" s="1" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="42" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="C12" s="42" t="s">
         <v>309</v>
       </c>
       <c r="D12" s="43"/>
       <c r="E12" s="1" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="42" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B13" s="41" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="C13" s="42" t="s">
         <v>313</v>
       </c>
       <c r="D13" s="43"/>
       <c r="E13" s="1" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="42" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B14" s="41" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="C14" s="42" t="s">
         <v>314</v>
       </c>
       <c r="D14" s="43"/>
       <c r="E14" s="1" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="42" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="C15" s="42" t="s">
         <v>315</v>
       </c>
       <c r="D15" s="43"/>
       <c r="E15" s="1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="42" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="C16" s="42" t="s">
         <v>316</v>
       </c>
       <c r="D16" s="43"/>
       <c r="E16" s="1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="42" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B17" s="41" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="C17" s="42" t="s">
         <v>311</v>
       </c>
       <c r="D17" s="43"/>
       <c r="E17" s="1" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="42" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B18" s="41" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="C18" s="43" t="s">
         <v>312</v>
       </c>
       <c r="D18" s="43"/>
       <c r="E18" s="1" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="42" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="C19" s="43" t="s">
         <v>359</v>
       </c>
       <c r="D19" s="43"/>
       <c r="E19" s="1" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="42" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="C20" s="42" t="s">
         <v>306</v>
       </c>
       <c r="D20" s="43"/>
       <c r="E20" s="12" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="42" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B21" s="41" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="C21" s="42" t="s">
         <v>307</v>
       </c>
       <c r="D21" s="43"/>
       <c r="E21" s="12" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B22" s="41" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="12" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B23" s="41" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="D23" s="43"/>
       <c r="E23" s="12" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B24" s="41" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="D24" s="43"/>
       <c r="E24" s="12" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B25" s="41"/>
       <c r="C25" s="43"/>
       <c r="D25" s="43"/>
       <c r="E25" s="12" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B26" s="41"/>
       <c r="C26" s="43"/>
       <c r="D26" s="43"/>
       <c r="E26" s="12" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B27" s="41"/>
       <c r="C27" s="43"/>
       <c r="D27" s="43"/>
       <c r="E27" s="12" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B28" s="41"/>
       <c r="C28" s="43"/>
       <c r="D28" s="43"/>
       <c r="E28" s="12" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B29" s="41"/>
       <c r="C29" s="43"/>
       <c r="D29" s="43"/>
       <c r="E29" s="12" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A30" s="42" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B30" s="41" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="12" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A31" s="42" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B31" s="41" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="D31" s="43"/>
       <c r="E31" s="12" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5491,188 +4490,188 @@
         <v>1</v>
       </c>
       <c r="B32" s="41" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="C32" s="43"/>
       <c r="D32" s="43"/>
       <c r="E32" s="1" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="B33" s="41" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="C33" s="43"/>
       <c r="D33" s="43"/>
       <c r="E33" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="B34" s="41" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="C34" s="43"/>
       <c r="D34" s="43"/>
       <c r="E34" s="12" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="C35" s="45" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="D35" s="45"/>
       <c r="E35" s="12" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B36" s="41" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="12" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B37" s="41" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="12" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B38" s="41" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="12" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B39" s="41" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="12" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B40" s="41" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="12" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B41" s="41" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="12" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B42" s="41" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="12" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B43" s="41" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="12" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B44" s="41" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="12" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
   </sheetData>
@@ -6220,10 +5219,10 @@
         <v>9999</v>
       </c>
       <c r="B2" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D2" s="37">
         <v>1080.152607223931</v>
@@ -6249,10 +5248,10 @@
         <v>9999</v>
       </c>
       <c r="B3" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C3" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D3" s="37">
         <v>23.777671918262815</v>
@@ -6278,10 +5277,10 @@
         <v>9999</v>
       </c>
       <c r="B4" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C4" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D4" s="37">
         <v>23.777671918262815</v>
@@ -6307,10 +5306,10 @@
         <v>9999</v>
       </c>
       <c r="B5" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C5" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D5" s="37">
         <v>722.95861675607034</v>
@@ -6336,10 +5335,10 @@
         <v>9999</v>
       </c>
       <c r="B6" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C6" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="D6" s="37">
         <v>722.95861675607034</v>
@@ -6365,10 +5364,10 @@
         <v>9999</v>
       </c>
       <c r="B7" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D7" s="37">
         <v>4365.4920119750241</v>
@@ -6394,7 +5393,7 @@
         <v>9999</v>
       </c>
       <c r="B8" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C8" t="s">
         <v>119</v>
@@ -6423,10 +5422,10 @@
         <v>9999</v>
       </c>
       <c r="B9" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C9" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D9" s="37">
         <v>0</v>
@@ -6452,10 +5451,10 @@
         <v>9999</v>
       </c>
       <c r="B10" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C10" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="D10" s="37">
         <v>0</v>
@@ -6481,10 +5480,10 @@
         <v>9999</v>
       </c>
       <c r="B11" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C11" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D11" s="37">
         <v>0</v>
@@ -6510,10 +5509,10 @@
         <v>9999</v>
       </c>
       <c r="B12" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C12" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D12" s="37">
         <v>67.190446389817993</v>
@@ -6539,10 +5538,10 @@
         <v>9999</v>
       </c>
       <c r="B13" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C13" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D13" s="37">
         <v>67.190446389817993</v>
@@ -6568,10 +5567,10 @@
         <v>9999</v>
       </c>
       <c r="B14" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D14" s="37">
         <v>830.3500214273206</v>
@@ -6597,10 +5596,10 @@
         <v>9999</v>
       </c>
       <c r="B15" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D15" s="37">
         <v>830.3500214273206</v>
@@ -6626,10 +5625,10 @@
         <v>9999</v>
       </c>
       <c r="B16" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C16" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D16" s="37">
         <v>830.3500214273206</v>
@@ -6655,10 +5654,10 @@
         <v>9999</v>
       </c>
       <c r="B17" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C17" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D17" s="37">
         <v>677.89857394760588</v>
@@ -6684,10 +5683,10 @@
         <v>9999</v>
       </c>
       <c r="B18" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C18" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D18" s="37">
         <v>677.89857394760588</v>
@@ -6713,10 +5712,10 @@
         <v>9999</v>
       </c>
       <c r="B19" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C19" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D19" s="37">
         <v>677.89857394760588</v>
@@ -6742,10 +5741,10 @@
         <v>9999</v>
       </c>
       <c r="B20" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C20" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D20" s="37">
         <v>528.52614620907616</v>
@@ -6771,10 +5770,10 @@
         <v>9999</v>
       </c>
       <c r="B21" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C21" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D21" s="37">
         <v>528.52614620907616</v>
@@ -6800,10 +5799,10 @@
         <v>9999</v>
       </c>
       <c r="B22" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C22" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D22" s="37">
         <v>528.52614620907616</v>
@@ -6829,10 +5828,10 @@
         <v>9999</v>
       </c>
       <c r="B23" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C23" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D23" s="37">
         <v>3234.9441989736843</v>
@@ -6858,10 +5857,10 @@
         <v>9999</v>
       </c>
       <c r="B24" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C24" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D24" s="37">
         <v>3234.9441989736843</v>
@@ -6887,10 +5886,10 @@
         <v>9999</v>
       </c>
       <c r="B25" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C25" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D25" s="37">
         <v>3234.9441989736843</v>
@@ -6916,7 +5915,7 @@
         <v>9999</v>
       </c>
       <c r="B26" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C26" t="s">
         <v>118</v>
@@ -6945,10 +5944,10 @@
         <v>9999</v>
       </c>
       <c r="B27" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C27" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D27" s="37">
         <v>1497.2287740322281</v>
@@ -6974,10 +5973,10 @@
         <v>9999</v>
       </c>
       <c r="B28" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C28" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D28" s="37">
         <v>56.227811725068918</v>
@@ -7003,7 +6002,7 @@
         <v>9999</v>
       </c>
       <c r="B29" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C29" t="s">
         <v>339</v>
@@ -7032,10 +6031,10 @@
         <v>9999</v>
       </c>
       <c r="B30" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C30" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D30" s="37">
         <v>83.46448226392279</v>
@@ -7061,10 +6060,10 @@
         <v>9999</v>
       </c>
       <c r="B31" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C31" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D31" s="37">
         <v>18.305586593676491</v>
@@ -7090,7 +6089,7 @@
         <v>9999</v>
       </c>
       <c r="B32" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C32" t="s">
         <v>338</v>
@@ -7119,10 +6118,10 @@
         <v>9999</v>
       </c>
       <c r="B33" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C33" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D33" s="37">
         <v>1.7053833345598797</v>
@@ -7148,10 +6147,10 @@
         <v>9999</v>
       </c>
       <c r="B34" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C34" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D34" s="37">
         <v>0.7317390810751</v>
@@ -7177,10 +6176,10 @@
         <v>9999</v>
       </c>
       <c r="B35" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C35" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="D35" s="37">
         <v>2091.3183488326904</v>
@@ -7206,10 +6205,10 @@
         <v>9999</v>
       </c>
       <c r="B36" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C36" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="D36" s="37">
         <v>2091.3183488326904</v>
@@ -7235,7 +6234,7 @@
         <v>9999</v>
       </c>
       <c r="B37" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C37" t="s">
         <v>159</v>
@@ -7264,7 +6263,7 @@
         <v>9999</v>
       </c>
       <c r="B38" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C38" t="s">
         <v>337</v>
@@ -7293,7 +6292,7 @@
         <v>9999</v>
       </c>
       <c r="B39" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C39" t="s">
         <v>300</v>
@@ -7322,10 +6321,10 @@
         <v>9999</v>
       </c>
       <c r="B40" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C40" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D40" s="37">
         <v>0.44478968664099999</v>
@@ -7351,7 +6350,7 @@
         <v>9999</v>
       </c>
       <c r="B41" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C41" t="s">
         <v>191</v>
@@ -7380,10 +6379,10 @@
         <v>9999</v>
       </c>
       <c r="B42" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C42" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D42" s="37">
         <v>149.69263234115053</v>
@@ -7409,7 +6408,7 @@
         <v>9999</v>
       </c>
       <c r="B43" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C43" t="s">
         <v>116</v>
@@ -7438,7 +6437,7 @@
         <v>9999</v>
       </c>
       <c r="B44" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C44" t="s">
         <v>117</v>
@@ -7467,7 +6466,7 @@
         <v>9999</v>
       </c>
       <c r="B45" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C45" t="s">
         <v>25</v>
@@ -7699,10 +6698,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="B2" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="C2">
         <v>214033</v>
@@ -8361,10 +7360,10 @@
     </row>
     <row r="4" spans="1:89" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="B4" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="C4">
         <v>214033</v>
@@ -8691,7 +7690,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>360</v>
@@ -8708,7 +7707,7 @@
         <v>214033</v>
       </c>
       <c r="C2" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="D2">
         <v>31.479347590500002</v>
@@ -8723,13 +7722,13 @@
         <v>214033</v>
       </c>
       <c r="H2" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="I2">
         <v>214033</v>
       </c>
       <c r="J2" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -15433,7 +14432,7 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:CI62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="AO12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
@@ -15744,7 +14743,7 @@
         <v>371</v>
       </c>
       <c r="CI4" s="1" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="5" spans="1:87" ht="39" x14ac:dyDescent="0.25">
@@ -22949,7 +21948,7 @@
     </row>
     <row r="51" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>22</v>
@@ -23298,7 +22297,7 @@
     <row r="52" spans="1:87" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="39"/>
       <c r="B52" s="1" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -23430,7 +22429,7 @@
     <row r="53" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A53" s="39"/>
       <c r="B53" s="1" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -23548,7 +22547,7 @@
     </row>
     <row r="54" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="17">
@@ -23791,7 +22790,7 @@
     </row>
     <row r="55" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="17">
@@ -24110,7 +23109,7 @@
     </row>
     <row r="57" spans="1:87" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C57" s="17">
         <v>300</v>
@@ -24238,13 +23237,13 @@
         <v>10</v>
       </c>
       <c r="AT57" s="2" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="AU57" s="2" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="AV57" s="2" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="AW57" s="17">
         <v>10.5</v>
@@ -24271,13 +23270,13 @@
         <v>8</v>
       </c>
       <c r="BE57" s="2" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="BF57" s="2" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="BG57" s="2" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="BH57" s="17">
         <v>19</v>
@@ -24316,7 +23315,7 @@
         <v>10.5</v>
       </c>
       <c r="BT57" s="2" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="BU57" s="17">
         <v>11</v>
@@ -24366,7 +23365,7 @@
     </row>
     <row r="58" spans="1:87" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C58" s="17">
         <f>0.5*(C57+C59)</f>
@@ -24684,7 +23683,7 @@
     </row>
     <row r="59" spans="1:87" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C59" s="17">
         <v>310</v>
@@ -24926,7 +23925,7 @@
     </row>
     <row r="60" spans="1:87" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C60" s="17">
         <v>310</v>
@@ -25168,7 +24167,7 @@
     </row>
     <row r="61" spans="1:87" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C61" s="17">
         <v>310</v>
@@ -25410,7 +24409,7 @@
     </row>
     <row r="62" spans="1:87" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C62" s="17">
         <v>310</v>

</xml_diff>